<commit_message>
MAJ NORMES FEV 25
</commit_message>
<xml_diff>
--- a/NORMES_NOV_24.xlsx
+++ b/NORMES_NOV_24.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="51" documentId="8_{2E579966-5A85-4B9D-AA96-30354E512A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0681D245-D9F3-4218-AB5E-2048BCBBF4AF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5 ans - 5 ans 11 mois" sheetId="1" r:id="rId1"/>
@@ -176,7 +176,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -287,7 +287,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4606,7 +4606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AH32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>

</xml_diff>